<commit_message>
complete for email job
</commit_message>
<xml_diff>
--- a/spring-boot-email-job-with-jira/src/main/resources/template/job_weekly_template.xlsx
+++ b/spring-boot-email-job-with-jira/src/main/resources/template/job_weekly_template.xlsx
@@ -26,6 +26,20 @@
     <author> </author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">jx:area(lastCell="i9")</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A4" authorId="0">
       <text>
         <r>
@@ -37,8 +51,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">jx:area(lastCell="H4")
-jx:each(items="currentWeekJobs" var="job" lastCell="H4")</t>
+          <t xml:space="preserve">jx:each(items="currentWeekJobs" var="job" lastCell="H4")</t>
         </r>
       </text>
     </comment>
@@ -53,8 +66,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">jx:area(lastCell="H8")
-jx:each(items="nextWeekJobs" var="job" lastCell="H8")</t>
+          <t xml:space="preserve">jx:each(items="nextWeekJobs" var="job" lastCell="H8")</t>
         </r>
       </text>
     </comment>
@@ -129,12 +141,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="YYYY\年M\月D&quot;日　&quot;DDDD&quot;, &quot;"/>
     <numFmt numFmtId="165" formatCode="0%"/>
     <numFmt numFmtId="166" formatCode="YYYY\年M\月D\日;\-;\-;@"/>
+    <numFmt numFmtId="167" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -168,6 +181,13 @@
       <sz val="12"/>
       <name val="微软雅黑"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -254,7 +274,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -297,6 +317,10 @@
     </xf>
     <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -318,8 +342,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -393,10 +417,10 @@
       <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -451,7 +475,7 @@
       <c r="A8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="11" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>